<commit_message>
feat: SVM in excel
</commit_message>
<xml_diff>
--- a/src/projects/svm-linear.xlsx
+++ b/src/projects/svm-linear.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelodeleon/ucu/2021-2/ML/UT4/TD/TD3/UT4_TA6-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FDD9CA-F8BE-E943-9B48-AD025957934A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FDEAEE-AB35-0543-9987-D620CED1FAD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24020" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t>X1</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>E15</t>
+  </si>
+  <si>
+    <t>Predicciones con Nuevo Dataset</t>
   </si>
 </sst>
 </file>
@@ -901,8 +904,381 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-UY"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>-1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$202:$A$206</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.9827311000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34442323000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1122223</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3334219999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.532233</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$202:$B$206</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.2343242999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2344439999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1233179999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.234348400000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1212398000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A258-0945-B881-D687922F4840}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$207:$A$211</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9.2344419999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.383449000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.2344439999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2337769999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.834111099999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$207:$B$211</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.7989633000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2332999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2383837999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.8888731999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2344439999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A258-0945-B881-D687922F4840}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1121236848"/>
+        <c:axId val="1106853088"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1121236848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-UY"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1106853088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1106853088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-UY"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1121236848"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1017,6 +1393,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2088,6 +2504,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2157,6 +3089,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>347134</xdr:colOff>
+      <xdr:row>197</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>728134</xdr:colOff>
+      <xdr:row>213</xdr:row>
+      <xdr:rowOff>46566</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16D9EF0A-80EF-604B-88A6-E14BF80C3C03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2486,10 +3454,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr published="0"/>
-  <dimension ref="A1:R197"/>
+  <dimension ref="A1:R211"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F202" sqref="F202"/>
+    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K217" sqref="K217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11059,7 +12027,7 @@
         <v>-1</v>
       </c>
       <c r="F188">
-        <f>IF(D188=E188,0,1)</f>
+        <f>F200</f>
         <v>0</v>
       </c>
       <c r="G188">
@@ -11159,7 +12127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A193">
         <v>7.8075211790000001</v>
       </c>
@@ -11182,7 +12150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A194">
         <v>6.1329981360000003</v>
       </c>
@@ -11205,7 +12173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A195">
         <v>7.5148293659999998</v>
       </c>
@@ -11228,7 +12196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A196">
         <v>5.502385039</v>
       </c>
@@ -11251,7 +12219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A197">
         <v>7.4329323650000001</v>
       </c>
@@ -11271,6 +12239,268 @@
       </c>
       <c r="F197">
         <f t="shared" si="166"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A200" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A201" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F201" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G201" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A202" s="2">
+        <v>2.9827311000000001</v>
+      </c>
+      <c r="B202">
+        <v>1.2343242999999999</v>
+      </c>
+      <c r="C202">
+        <f>$A$184*A202+B202*$B$184</f>
+        <v>0.73779643066482969</v>
+      </c>
+      <c r="D202">
+        <f>IF(C202&lt;0,-1,1)</f>
+        <v>1</v>
+      </c>
+      <c r="E202">
+        <v>-1</v>
+      </c>
+      <c r="F202">
+        <f>IF(D202=E202,0,1)</f>
+        <v>1</v>
+      </c>
+      <c r="G202">
+        <f>(1-(SUM(F202:F211)/COUNT(F202:F211)))*100</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A203">
+        <v>0.34442323000000002</v>
+      </c>
+      <c r="B203">
+        <v>3.2344439999999999</v>
+      </c>
+      <c r="C203">
+        <f t="shared" ref="C203:C211" si="167">$A$184*A203+B203*$B$184</f>
+        <v>-2.1519600566477299</v>
+      </c>
+      <c r="D203">
+        <f t="shared" ref="D203:D211" si="168">IF(C203&lt;0,-1,1)</f>
+        <v>-1</v>
+      </c>
+      <c r="E203">
+        <v>-1</v>
+      </c>
+      <c r="F203">
+        <f t="shared" ref="F203:F211" si="169">IF(D203=E203,0,1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A204">
+        <v>2.1122223</v>
+      </c>
+      <c r="B204">
+        <v>3.1233179999999998</v>
+      </c>
+      <c r="C204">
+        <f t="shared" si="167"/>
+        <v>-1.1049608670002209</v>
+      </c>
+      <c r="D204">
+        <f t="shared" si="168"/>
+        <v>-1</v>
+      </c>
+      <c r="E204">
+        <v>-1</v>
+      </c>
+      <c r="F204">
+        <f t="shared" si="169"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A205">
+        <v>5.3334219999999997</v>
+      </c>
+      <c r="B205">
+        <v>33.234348400000002</v>
+      </c>
+      <c r="C205">
+        <f t="shared" si="167"/>
+        <v>-21.130526443084385</v>
+      </c>
+      <c r="D205">
+        <f t="shared" si="168"/>
+        <v>-1</v>
+      </c>
+      <c r="E205">
+        <v>-1</v>
+      </c>
+      <c r="F205">
+        <f t="shared" si="169"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A206">
+        <v>1.532233</v>
+      </c>
+      <c r="B206">
+        <v>3.1212398000000001</v>
+      </c>
+      <c r="C206">
+        <f t="shared" si="167"/>
+        <v>-1.4205826696163628</v>
+      </c>
+      <c r="D206">
+        <f t="shared" si="168"/>
+        <v>-1</v>
+      </c>
+      <c r="E206">
+        <v>-1</v>
+      </c>
+      <c r="F206">
+        <f t="shared" si="169"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A207">
+        <v>9.2344419999999996</v>
+      </c>
+      <c r="B207">
+        <v>8.7989633000000005</v>
+      </c>
+      <c r="C207">
+        <f t="shared" si="167"/>
+        <v>-1.3173019169310871</v>
+      </c>
+      <c r="D207">
+        <f t="shared" si="168"/>
+        <v>-1</v>
+      </c>
+      <c r="E207">
+        <v>1</v>
+      </c>
+      <c r="F207">
+        <f t="shared" si="169"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A208">
+        <v>11.383449000000001</v>
+      </c>
+      <c r="B208">
+        <v>2.2332999999999998</v>
+      </c>
+      <c r="C208">
+        <f t="shared" si="167"/>
+        <v>4.6083163071849098</v>
+      </c>
+      <c r="D208">
+        <f t="shared" si="168"/>
+        <v>1</v>
+      </c>
+      <c r="E208">
+        <v>1</v>
+      </c>
+      <c r="F208">
+        <f t="shared" si="169"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A209">
+        <v>6.2344439999999999</v>
+      </c>
+      <c r="B209">
+        <v>3.2383837999999998</v>
+      </c>
+      <c r="C209">
+        <f t="shared" si="167"/>
+        <v>1.0657240462517339</v>
+      </c>
+      <c r="D209">
+        <f t="shared" si="168"/>
+        <v>1</v>
+      </c>
+      <c r="E209">
+        <v>1</v>
+      </c>
+      <c r="F209">
+        <f t="shared" si="169"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A210">
+        <v>5.2337769999999999</v>
+      </c>
+      <c r="B210">
+        <v>7.8888731999999999</v>
+      </c>
+      <c r="C210">
+        <f t="shared" si="167"/>
+        <v>-2.8462821531279445</v>
+      </c>
+      <c r="D210">
+        <f t="shared" si="168"/>
+        <v>-1</v>
+      </c>
+      <c r="E210">
+        <v>1</v>
+      </c>
+      <c r="F210">
+        <f t="shared" si="169"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A211">
+        <v>10.834111099999999</v>
+      </c>
+      <c r="B211">
+        <v>4.2344439999999999</v>
+      </c>
+      <c r="C211">
+        <f t="shared" si="167"/>
+        <v>2.8600218535324955</v>
+      </c>
+      <c r="D211">
+        <f t="shared" si="168"/>
+        <v>1</v>
+      </c>
+      <c r="E211">
+        <v>1</v>
+      </c>
+      <c r="F211">
+        <f t="shared" si="169"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>